<commit_message>
Updated DL-based with T5 model
</commit_message>
<xml_diff>
--- a/xls/Four_Recommendations_evaluation.xlsx
+++ b/xls/Four_Recommendations_evaluation.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10711"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10111"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://usi365-my.sharepoint.com/personal/cinism_usi_ch/Documents/code/004_Characteristic_Of_Code_Replication_Package/Website/ICSE22_replication/xls/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://usi365-my.sharepoint.com/personal/cinism_usi_ch/Documents/code/004_Characteristic_Of_Code_Replication_Package/Website/code-recommenders.github.io/xls/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="339" documentId="11_2D8FB22614D9856A75BAC250946EE48913096B0A" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{6ED8D4E1-F531-8C4D-A365-78D9B6271BC2}"/>
+  <xr:revisionPtr revIDLastSave="343" documentId="11_2D8FB22614D9856A75BAC250946EE48913096B0A" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F310EB0E-037B-B64D-9742-F220CD1AABC3}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="35840" windowHeight="21940" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -117,13 +117,13 @@
     <t>Retrieval-based Code Completion</t>
   </si>
   <si>
-    <t>DL-based Code Completion</t>
-  </si>
-  <si>
     <t>Natural Language to Code Translation</t>
   </si>
   <si>
     <t>IDE Code Completion</t>
+  </si>
+  <si>
+    <t>T5 model</t>
   </si>
 </sst>
 </file>
@@ -526,7 +526,7 @@
   <dimension ref="A1:BB241"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:B1048576"/>
+      <selection activeCell="B70" sqref="B70"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -683,7 +683,7 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="C3" t="s">
         <v>24</v>
@@ -740,7 +740,7 @@
         <v>1</v>
       </c>
       <c r="B4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C4" t="s">
         <v>17</v>
@@ -797,7 +797,7 @@
         <v>1</v>
       </c>
       <c r="B5" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="C5" t="s">
         <v>24</v>
@@ -854,7 +854,7 @@
         <v>1</v>
       </c>
       <c r="B6" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C6" t="s">
         <v>24</v>
@@ -911,7 +911,7 @@
         <v>1</v>
       </c>
       <c r="B7" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C7" t="s">
         <v>24</v>
@@ -1025,7 +1025,7 @@
         <v>1</v>
       </c>
       <c r="B9" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C9" t="s">
         <v>24</v>
@@ -1082,7 +1082,7 @@
         <v>1</v>
       </c>
       <c r="B10" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="C10" t="s">
         <v>17</v>
@@ -1139,7 +1139,7 @@
         <v>1</v>
       </c>
       <c r="B11" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C11" t="s">
         <v>24</v>
@@ -1196,7 +1196,7 @@
         <v>1</v>
       </c>
       <c r="B12" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="C12" t="s">
         <v>17</v>
@@ -1253,7 +1253,7 @@
         <v>1</v>
       </c>
       <c r="B13" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C13" t="s">
         <v>24</v>
@@ -1310,7 +1310,7 @@
         <v>2</v>
       </c>
       <c r="B14" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C14" t="s">
         <v>17</v>
@@ -1424,7 +1424,7 @@
         <v>2</v>
       </c>
       <c r="B16" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C16" t="s">
         <v>17</v>
@@ -1538,7 +1538,7 @@
         <v>2</v>
       </c>
       <c r="B18" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C18" t="s">
         <v>17</v>
@@ -1594,7 +1594,7 @@
         <v>2</v>
       </c>
       <c r="B19" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C19" t="s">
         <v>24</v>
@@ -1650,7 +1650,7 @@
         <v>2</v>
       </c>
       <c r="B20" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="C20" t="s">
         <v>17</v>
@@ -1874,7 +1874,7 @@
         <v>2</v>
       </c>
       <c r="B24" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C24" t="s">
         <v>24</v>
@@ -1930,7 +1930,7 @@
         <v>2</v>
       </c>
       <c r="B25" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="C25" t="s">
         <v>17</v>
@@ -1986,7 +1986,7 @@
         <v>2</v>
       </c>
       <c r="B26" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C26" t="s">
         <v>24</v>
@@ -2098,7 +2098,7 @@
         <v>3</v>
       </c>
       <c r="B28" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C28" t="s">
         <v>24</v>
@@ -2154,7 +2154,7 @@
         <v>3</v>
       </c>
       <c r="B29" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C29" t="s">
         <v>24</v>
@@ -2210,7 +2210,7 @@
         <v>3</v>
       </c>
       <c r="B30" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="C30" t="s">
         <v>17</v>
@@ -2266,7 +2266,7 @@
         <v>3</v>
       </c>
       <c r="B31" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C31" t="s">
         <v>24</v>
@@ -2322,7 +2322,7 @@
         <v>3</v>
       </c>
       <c r="B32" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C32" t="s">
         <v>24</v>
@@ -2378,7 +2378,7 @@
         <v>3</v>
       </c>
       <c r="B33" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="C33" t="s">
         <v>17</v>
@@ -2434,7 +2434,7 @@
         <v>3</v>
       </c>
       <c r="B34" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C34" t="s">
         <v>24</v>
@@ -2490,7 +2490,7 @@
         <v>3</v>
       </c>
       <c r="B35" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="C35" t="s">
         <v>17</v>
@@ -2602,7 +2602,7 @@
         <v>4</v>
       </c>
       <c r="B37" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C37" t="s">
         <v>24</v>
@@ -2714,7 +2714,7 @@
         <v>4</v>
       </c>
       <c r="B39" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="C39" t="s">
         <v>17</v>
@@ -2826,7 +2826,7 @@
         <v>4</v>
       </c>
       <c r="B41" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C41" t="s">
         <v>24</v>
@@ -2882,7 +2882,7 @@
         <v>4</v>
       </c>
       <c r="B42" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C42" t="s">
         <v>24</v>
@@ -2938,7 +2938,7 @@
         <v>4</v>
       </c>
       <c r="B43" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="C43" t="s">
         <v>24</v>
@@ -2994,7 +2994,7 @@
         <v>5</v>
       </c>
       <c r="B44" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="C44" t="s">
         <v>17</v>
@@ -3050,7 +3050,7 @@
         <v>5</v>
       </c>
       <c r="B45" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C45" t="s">
         <v>24</v>
@@ -3106,7 +3106,7 @@
         <v>5</v>
       </c>
       <c r="B46" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="C46" t="s">
         <v>17</v>
@@ -3162,7 +3162,7 @@
         <v>5</v>
       </c>
       <c r="B47" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C47" t="s">
         <v>24</v>
@@ -3218,7 +3218,7 @@
         <v>6</v>
       </c>
       <c r="B48" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C48" t="s">
         <v>17</v>
@@ -3274,7 +3274,7 @@
         <v>6</v>
       </c>
       <c r="B49" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C49" t="s">
         <v>24</v>
@@ -3330,7 +3330,7 @@
         <v>6</v>
       </c>
       <c r="B50" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="C50" t="s">
         <v>24</v>
@@ -3386,7 +3386,7 @@
         <v>6</v>
       </c>
       <c r="B51" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="C51" t="s">
         <v>24</v>
@@ -3442,7 +3442,7 @@
         <v>6</v>
       </c>
       <c r="B52" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="C52" t="s">
         <v>17</v>
@@ -3610,7 +3610,7 @@
         <v>6</v>
       </c>
       <c r="B55" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C55" t="s">
         <v>17</v>
@@ -3666,7 +3666,7 @@
         <v>6</v>
       </c>
       <c r="B56" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C56" t="s">
         <v>24</v>
@@ -3722,7 +3722,7 @@
         <v>6</v>
       </c>
       <c r="B57" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C57" t="s">
         <v>24</v>
@@ -3778,7 +3778,7 @@
         <v>6</v>
       </c>
       <c r="B58" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C58" t="s">
         <v>17</v>
@@ -3834,7 +3834,7 @@
         <v>6</v>
       </c>
       <c r="B59" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="C59" t="s">
         <v>24</v>
@@ -3890,7 +3890,7 @@
         <v>7</v>
       </c>
       <c r="B60" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="C60" t="s">
         <v>24</v>
@@ -3946,7 +3946,7 @@
         <v>7</v>
       </c>
       <c r="B61" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C61" t="s">
         <v>24</v>
@@ -4058,7 +4058,7 @@
         <v>7</v>
       </c>
       <c r="B63" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="C63" t="s">
         <v>24</v>
@@ -4170,7 +4170,7 @@
         <v>8</v>
       </c>
       <c r="B65" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="C65" t="s">
         <v>17</v>
@@ -4226,7 +4226,7 @@
         <v>8</v>
       </c>
       <c r="B66" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C66" t="s">
         <v>24</v>
@@ -4282,7 +4282,7 @@
         <v>8</v>
       </c>
       <c r="B67" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="C67" t="s">
         <v>17</v>
@@ -4338,7 +4338,7 @@
         <v>8</v>
       </c>
       <c r="B68" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C68" t="s">
         <v>24</v>
@@ -4394,7 +4394,7 @@
         <v>8</v>
       </c>
       <c r="B69" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C69" t="s">
         <v>24</v>
@@ -4450,7 +4450,7 @@
         <v>8</v>
       </c>
       <c r="B70" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="C70" t="s">
         <v>17</v>
@@ -4562,7 +4562,7 @@
         <v>8</v>
       </c>
       <c r="B72" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="C72" t="s">
         <v>24</v>
@@ -4618,7 +4618,7 @@
         <v>8</v>
       </c>
       <c r="B73" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="C73" t="s">
         <v>17</v>
@@ -4674,7 +4674,7 @@
         <v>8</v>
       </c>
       <c r="B74" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C74" t="s">
         <v>24</v>
@@ -4730,7 +4730,7 @@
         <v>9</v>
       </c>
       <c r="B75" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C75" t="s">
         <v>17</v>
@@ -4842,7 +4842,7 @@
         <v>9</v>
       </c>
       <c r="B77" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="C77" t="s">
         <v>24</v>
@@ -4954,7 +4954,7 @@
         <v>9</v>
       </c>
       <c r="B79" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="C79" t="s">
         <v>24</v>
@@ -5066,7 +5066,7 @@
         <v>9</v>
       </c>
       <c r="B81" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C81" t="s">
         <v>24</v>
@@ -5122,7 +5122,7 @@
         <v>9</v>
       </c>
       <c r="B82" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="C82" t="s">
         <v>17</v>
@@ -5178,7 +5178,7 @@
         <v>9</v>
       </c>
       <c r="B83" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C83" t="s">
         <v>24</v>
@@ -5234,7 +5234,7 @@
         <v>10</v>
       </c>
       <c r="B84" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C84" t="s">
         <v>17</v>
@@ -5290,7 +5290,7 @@
         <v>10</v>
       </c>
       <c r="B85" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="C85" t="s">
         <v>24</v>
@@ -5346,7 +5346,7 @@
         <v>10</v>
       </c>
       <c r="B86" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C86" t="s">
         <v>24</v>
@@ -5402,7 +5402,7 @@
         <v>10</v>
       </c>
       <c r="B87" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="C87" t="s">
         <v>17</v>
@@ -5514,7 +5514,7 @@
         <v>10</v>
       </c>
       <c r="B89" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C89" t="s">
         <v>24</v>
@@ -5570,7 +5570,7 @@
         <v>10</v>
       </c>
       <c r="B90" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="C90" t="s">
         <v>24</v>
@@ -5682,7 +5682,7 @@
         <v>10</v>
       </c>
       <c r="B92" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C92" t="s">
         <v>17</v>
@@ -5794,7 +5794,7 @@
         <v>10</v>
       </c>
       <c r="B94" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C94" t="s">
         <v>17</v>
@@ -5850,7 +5850,7 @@
         <v>10</v>
       </c>
       <c r="B95" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="C95" t="s">
         <v>24</v>
@@ -5906,7 +5906,7 @@
         <v>11</v>
       </c>
       <c r="B96" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="C96" t="s">
         <v>17</v>
@@ -6018,7 +6018,7 @@
         <v>11</v>
       </c>
       <c r="B98" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="C98" t="s">
         <v>17</v>
@@ -6074,7 +6074,7 @@
         <v>11</v>
       </c>
       <c r="B99" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C99" t="s">
         <v>24</v>
@@ -6130,7 +6130,7 @@
         <v>11</v>
       </c>
       <c r="B100" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="C100" t="s">
         <v>17</v>
@@ -6186,7 +6186,7 @@
         <v>11</v>
       </c>
       <c r="B101" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C101" t="s">
         <v>24</v>
@@ -6242,7 +6242,7 @@
         <v>11</v>
       </c>
       <c r="B102" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="C102" t="s">
         <v>17</v>
@@ -6298,7 +6298,7 @@
         <v>11</v>
       </c>
       <c r="B103" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C103" t="s">
         <v>24</v>
@@ -6354,7 +6354,7 @@
         <v>11</v>
       </c>
       <c r="B104" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="C104" t="s">
         <v>17</v>
@@ -6410,7 +6410,7 @@
         <v>11</v>
       </c>
       <c r="B105" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C105" t="s">
         <v>24</v>
@@ -6466,7 +6466,7 @@
         <v>12</v>
       </c>
       <c r="B106" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C106" t="s">
         <v>17</v>
@@ -6522,7 +6522,7 @@
         <v>12</v>
       </c>
       <c r="B107" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="C107" t="s">
         <v>24</v>
@@ -6578,7 +6578,7 @@
         <v>12</v>
       </c>
       <c r="B108" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C108" t="s">
         <v>17</v>
@@ -6690,7 +6690,7 @@
         <v>12</v>
       </c>
       <c r="B110" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="C110" t="s">
         <v>17</v>
@@ -6746,7 +6746,7 @@
         <v>12</v>
       </c>
       <c r="B111" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C111" t="s">
         <v>24</v>
@@ -6858,7 +6858,7 @@
         <v>13</v>
       </c>
       <c r="B113" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="C113" t="s">
         <v>17</v>
@@ -6970,7 +6970,7 @@
         <v>13</v>
       </c>
       <c r="B115" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="C115" t="s">
         <v>17</v>
@@ -7082,7 +7082,7 @@
         <v>13</v>
       </c>
       <c r="B117" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="C117" t="s">
         <v>17</v>
@@ -7138,7 +7138,7 @@
         <v>13</v>
       </c>
       <c r="B118" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C118" t="s">
         <v>24</v>
@@ -7194,7 +7194,7 @@
         <v>13</v>
       </c>
       <c r="B119" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="C119" t="s">
         <v>17</v>
@@ -7250,7 +7250,7 @@
         <v>13</v>
       </c>
       <c r="B120" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C120" t="s">
         <v>24</v>
@@ -7306,7 +7306,7 @@
         <v>13</v>
       </c>
       <c r="B121" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="C121" t="s">
         <v>17</v>
@@ -7362,7 +7362,7 @@
         <v>13</v>
       </c>
       <c r="B122" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C122" t="s">
         <v>24</v>
@@ -7418,7 +7418,7 @@
         <v>13</v>
       </c>
       <c r="B123" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="C123" t="s">
         <v>17</v>
@@ -7474,7 +7474,7 @@
         <v>13</v>
       </c>
       <c r="B124" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C124" t="s">
         <v>24</v>
@@ -7586,7 +7586,7 @@
         <v>14</v>
       </c>
       <c r="B126" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C126" t="s">
         <v>24</v>
@@ -7642,7 +7642,7 @@
         <v>14</v>
       </c>
       <c r="B127" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="C127" t="s">
         <v>17</v>
@@ -7698,7 +7698,7 @@
         <v>14</v>
       </c>
       <c r="B128" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C128" t="s">
         <v>24</v>
@@ -7754,7 +7754,7 @@
         <v>14</v>
       </c>
       <c r="B129" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="C129" t="s">
         <v>17</v>
@@ -7810,7 +7810,7 @@
         <v>14</v>
       </c>
       <c r="B130" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C130" t="s">
         <v>24</v>
@@ -7866,7 +7866,7 @@
         <v>15</v>
       </c>
       <c r="B131" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="C131" t="s">
         <v>17</v>
@@ -7978,7 +7978,7 @@
         <v>15</v>
       </c>
       <c r="B133" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="C133" t="s">
         <v>17</v>
@@ -8034,7 +8034,7 @@
         <v>15</v>
       </c>
       <c r="B134" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C134" t="s">
         <v>24</v>
@@ -8090,7 +8090,7 @@
         <v>15</v>
       </c>
       <c r="B135" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="C135" t="s">
         <v>17</v>
@@ -8146,7 +8146,7 @@
         <v>15</v>
       </c>
       <c r="B136" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C136" t="s">
         <v>24</v>
@@ -8202,7 +8202,7 @@
         <v>16</v>
       </c>
       <c r="B137" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C137" t="s">
         <v>17</v>
@@ -8258,7 +8258,7 @@
         <v>16</v>
       </c>
       <c r="B138" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C138" t="s">
         <v>24</v>
@@ -8314,7 +8314,7 @@
         <v>16</v>
       </c>
       <c r="B139" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C139" t="s">
         <v>24</v>
@@ -8370,7 +8370,7 @@
         <v>16</v>
       </c>
       <c r="B140" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C140" t="s">
         <v>17</v>
@@ -8426,7 +8426,7 @@
         <v>16</v>
       </c>
       <c r="B141" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C141" t="s">
         <v>24</v>
@@ -8482,7 +8482,7 @@
         <v>16</v>
       </c>
       <c r="B142" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C142" t="s">
         <v>24</v>
@@ -8538,7 +8538,7 @@
         <v>16</v>
       </c>
       <c r="B143" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="C143" t="s">
         <v>24</v>
@@ -8594,7 +8594,7 @@
         <v>16</v>
       </c>
       <c r="B144" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C144" t="s">
         <v>17</v>
@@ -8650,7 +8650,7 @@
         <v>16</v>
       </c>
       <c r="B145" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="C145" t="s">
         <v>24</v>
@@ -8706,7 +8706,7 @@
         <v>16</v>
       </c>
       <c r="B146" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C146" t="s">
         <v>17</v>
@@ -8762,7 +8762,7 @@
         <v>16</v>
       </c>
       <c r="B147" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="C147" t="s">
         <v>24</v>
@@ -8818,7 +8818,7 @@
         <v>17</v>
       </c>
       <c r="B148" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C148" t="s">
         <v>17</v>
@@ -8874,7 +8874,7 @@
         <v>17</v>
       </c>
       <c r="B149" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C149" t="s">
         <v>24</v>
@@ -8930,7 +8930,7 @@
         <v>17</v>
       </c>
       <c r="B150" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C150" t="s">
         <v>17</v>
@@ -9098,7 +9098,7 @@
         <v>17</v>
       </c>
       <c r="B153" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="C153" t="s">
         <v>24</v>
@@ -9210,7 +9210,7 @@
         <v>17</v>
       </c>
       <c r="B155" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C155" t="s">
         <v>24</v>
@@ -9322,7 +9322,7 @@
         <v>18</v>
       </c>
       <c r="B157" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C157" t="s">
         <v>24</v>
@@ -9378,7 +9378,7 @@
         <v>18</v>
       </c>
       <c r="B158" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="C158" t="s">
         <v>24</v>
@@ -9434,7 +9434,7 @@
         <v>19</v>
       </c>
       <c r="B159" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="C159" t="s">
         <v>17</v>
@@ -9490,7 +9490,7 @@
         <v>19</v>
       </c>
       <c r="B160" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C160" t="s">
         <v>24</v>
@@ -9546,7 +9546,7 @@
         <v>19</v>
       </c>
       <c r="B161" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="C161" t="s">
         <v>17</v>
@@ -9714,7 +9714,7 @@
         <v>19</v>
       </c>
       <c r="B164" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="C164" t="s">
         <v>17</v>
@@ -9770,7 +9770,7 @@
         <v>19</v>
       </c>
       <c r="B165" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C165" t="s">
         <v>24</v>
@@ -9826,7 +9826,7 @@
         <v>19</v>
       </c>
       <c r="B166" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C166" t="s">
         <v>24</v>
@@ -9882,7 +9882,7 @@
         <v>19</v>
       </c>
       <c r="B167" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="C167" t="s">
         <v>17</v>
@@ -9938,7 +9938,7 @@
         <v>19</v>
       </c>
       <c r="B168" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C168" t="s">
         <v>24</v>
@@ -9994,7 +9994,7 @@
         <v>19</v>
       </c>
       <c r="B169" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="C169" t="s">
         <v>17</v>
@@ -10106,7 +10106,7 @@
         <v>19</v>
       </c>
       <c r="B171" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="C171" t="s">
         <v>17</v>
@@ -10162,7 +10162,7 @@
         <v>19</v>
       </c>
       <c r="B172" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C172" t="s">
         <v>24</v>
@@ -10218,7 +10218,7 @@
         <v>19</v>
       </c>
       <c r="B173" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="C173" t="s">
         <v>17</v>
@@ -10274,7 +10274,7 @@
         <v>19</v>
       </c>
       <c r="B174" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C174" t="s">
         <v>24</v>
@@ -10330,7 +10330,7 @@
         <v>20</v>
       </c>
       <c r="B175" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C175" t="s">
         <v>24</v>
@@ -10386,7 +10386,7 @@
         <v>20</v>
       </c>
       <c r="B176" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="C176" t="s">
         <v>24</v>
@@ -10442,7 +10442,7 @@
         <v>21</v>
       </c>
       <c r="B177" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C177" t="s">
         <v>24</v>
@@ -10498,7 +10498,7 @@
         <v>21</v>
       </c>
       <c r="B178" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C178" t="s">
         <v>24</v>
@@ -10610,7 +10610,7 @@
         <v>21</v>
       </c>
       <c r="B180" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C180" t="s">
         <v>17</v>
@@ -10666,7 +10666,7 @@
         <v>21</v>
       </c>
       <c r="B181" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="C181" t="s">
         <v>24</v>
@@ -10722,7 +10722,7 @@
         <v>22</v>
       </c>
       <c r="B182" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C182" t="s">
         <v>17</v>
@@ -10778,7 +10778,7 @@
         <v>22</v>
       </c>
       <c r="B183" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="C183" t="s">
         <v>24</v>
@@ -10890,7 +10890,7 @@
         <v>22</v>
       </c>
       <c r="B185" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C185" t="s">
         <v>24</v>
@@ -10946,7 +10946,7 @@
         <v>23</v>
       </c>
       <c r="B186" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="C186" t="s">
         <v>17</v>
@@ -11058,7 +11058,7 @@
         <v>23</v>
       </c>
       <c r="B188" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C188" t="s">
         <v>17</v>
@@ -11114,7 +11114,7 @@
         <v>23</v>
       </c>
       <c r="B189" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="C189" t="s">
         <v>24</v>
@@ -11170,7 +11170,7 @@
         <v>23</v>
       </c>
       <c r="B190" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="C190" t="s">
         <v>17</v>
@@ -11226,7 +11226,7 @@
         <v>23</v>
       </c>
       <c r="B191" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C191" t="s">
         <v>24</v>
@@ -11338,7 +11338,7 @@
         <v>24</v>
       </c>
       <c r="B193" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C193" t="s">
         <v>24</v>
@@ -11394,7 +11394,7 @@
         <v>24</v>
       </c>
       <c r="B194" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="C194" t="s">
         <v>17</v>
@@ -11506,7 +11506,7 @@
         <v>24</v>
       </c>
       <c r="B196" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="C196" t="s">
         <v>17</v>
@@ -11562,7 +11562,7 @@
         <v>24</v>
       </c>
       <c r="B197" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C197" t="s">
         <v>24</v>
@@ -11618,7 +11618,7 @@
         <v>24</v>
       </c>
       <c r="B198" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="C198" t="s">
         <v>17</v>
@@ -11674,7 +11674,7 @@
         <v>24</v>
       </c>
       <c r="B199" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="C199" t="s">
         <v>17</v>
@@ -11730,7 +11730,7 @@
         <v>25</v>
       </c>
       <c r="B200" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="C200" t="s">
         <v>24</v>
@@ -11786,7 +11786,7 @@
         <v>25</v>
       </c>
       <c r="B201" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C201" t="s">
         <v>24</v>
@@ -11898,7 +11898,7 @@
         <v>25</v>
       </c>
       <c r="B203" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="C203" t="s">
         <v>17</v>
@@ -11954,7 +11954,7 @@
         <v>25</v>
       </c>
       <c r="B204" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C204" t="s">
         <v>24</v>
@@ -12010,7 +12010,7 @@
         <v>26</v>
       </c>
       <c r="B205" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="C205" t="s">
         <v>24</v>
@@ -12066,7 +12066,7 @@
         <v>26</v>
       </c>
       <c r="B206" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="C206" t="s">
         <v>24</v>
@@ -12122,7 +12122,7 @@
         <v>26</v>
       </c>
       <c r="B207" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="C207" t="s">
         <v>24</v>
@@ -12234,7 +12234,7 @@
         <v>26</v>
       </c>
       <c r="B209" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C209" t="s">
         <v>24</v>
@@ -12290,7 +12290,7 @@
         <v>26</v>
       </c>
       <c r="B210" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="C210" t="s">
         <v>24</v>
@@ -12346,7 +12346,7 @@
         <v>26</v>
       </c>
       <c r="B211" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="C211" t="s">
         <v>24</v>
@@ -12402,7 +12402,7 @@
         <v>26</v>
       </c>
       <c r="B212" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="C212" t="s">
         <v>17</v>
@@ -12514,7 +12514,7 @@
         <v>27</v>
       </c>
       <c r="B214" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C214" t="s">
         <v>17</v>
@@ -12570,7 +12570,7 @@
         <v>27</v>
       </c>
       <c r="B215" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C215" t="s">
         <v>24</v>
@@ -12626,7 +12626,7 @@
         <v>27</v>
       </c>
       <c r="B216" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C216" t="s">
         <v>17</v>
@@ -12682,7 +12682,7 @@
         <v>27</v>
       </c>
       <c r="B217" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C217" t="s">
         <v>24</v>
@@ -12794,7 +12794,7 @@
         <v>28</v>
       </c>
       <c r="B219" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C219" t="s">
         <v>24</v>
@@ -12850,7 +12850,7 @@
         <v>28</v>
       </c>
       <c r="B220" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="C220" t="s">
         <v>17</v>
@@ -12906,7 +12906,7 @@
         <v>28</v>
       </c>
       <c r="B221" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C221" t="s">
         <v>24</v>
@@ -12962,7 +12962,7 @@
         <v>28</v>
       </c>
       <c r="B222" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="C222" t="s">
         <v>17</v>
@@ -13130,7 +13130,7 @@
         <v>29</v>
       </c>
       <c r="B225" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="C225" t="s">
         <v>17</v>
@@ -13242,7 +13242,7 @@
         <v>29</v>
       </c>
       <c r="B227" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="C227" t="s">
         <v>24</v>
@@ -13298,7 +13298,7 @@
         <v>30</v>
       </c>
       <c r="B228" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="C228" t="s">
         <v>17</v>
@@ -13354,7 +13354,7 @@
         <v>30</v>
       </c>
       <c r="B229" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C229" t="s">
         <v>24</v>
@@ -13410,7 +13410,7 @@
         <v>30</v>
       </c>
       <c r="B230" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C230" t="s">
         <v>17</v>
@@ -13466,7 +13466,7 @@
         <v>30</v>
       </c>
       <c r="B231" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="C231" t="s">
         <v>24</v>
@@ -13522,7 +13522,7 @@
         <v>30</v>
       </c>
       <c r="B232" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C232" t="s">
         <v>17</v>
@@ -13578,7 +13578,7 @@
         <v>30</v>
       </c>
       <c r="B233" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C233" t="s">
         <v>24</v>
@@ -13634,7 +13634,7 @@
         <v>30</v>
       </c>
       <c r="B234" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="C234" t="s">
         <v>17</v>
@@ -13746,7 +13746,7 @@
         <v>30</v>
       </c>
       <c r="B236" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="C236" t="s">
         <v>17</v>
@@ -13802,7 +13802,7 @@
         <v>30</v>
       </c>
       <c r="B237" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C237" t="s">
         <v>24</v>
@@ -13858,7 +13858,7 @@
         <v>30</v>
       </c>
       <c r="B238" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="C238" t="s">
         <v>17</v>
@@ -13914,7 +13914,7 @@
         <v>30</v>
       </c>
       <c r="B239" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C239" t="s">
         <v>24</v>
@@ -13970,7 +13970,7 @@
         <v>30</v>
       </c>
       <c r="B240" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C240" t="s">
         <v>17</v>
@@ -14026,7 +14026,7 @@
         <v>30</v>
       </c>
       <c r="B241" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="C241" t="s">
         <v>24</v>

</xml_diff>